<commit_message>
Fix Excel refresh: Use deployed Excel file with cache busting
</commit_message>
<xml_diff>
--- a/Customer Capital Work Tracker-2.xlsx
+++ b/Customer Capital Work Tracker-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatanathandwarakanathan/Desktop/CC-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944BFB34-A4AD-994B-9B68-E185D780F4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2485556D-3EB8-C749-B610-DE6F3F794F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25720" windowHeight="12980" xr2:uid="{0A6F300E-DE9E-4F51-9C84-70C237940D4C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
   <si>
     <t>S#</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>RAG - Learning Agent</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -626,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8563BA6-12A6-4529-B2F8-0C9B569F1FE6}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -788,7 +791,9 @@
       <c r="E6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="F6" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G6" s="4" t="s">
         <v>24</v>
       </c>
@@ -812,7 +817,9 @@
       <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="12"/>
+      <c r="F7" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G7" s="4" t="s">
         <v>9</v>
       </c>
@@ -836,7 +843,9 @@
       <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="12"/>
+      <c r="F8" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="3" t="s">
         <v>16</v>
@@ -858,7 +867,9 @@
       <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G9" s="4" t="s">
         <v>22</v>
       </c>
@@ -1034,7 +1045,9 @@
         <v>13</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="12"/>
+      <c r="F16" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G16" s="4"/>
       <c r="H16" s="3" t="s">
         <v>46</v>

</xml_diff>